<commit_message>
Move Observed tab to front so it diffs with previous version
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/Lincoln2021.xlsx
+++ b/Tests/Validation/Wheat/data/Lincoln2021.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51749308-1A8C-4174-ACDD-9867ACA312E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291C718A-974A-44E6-92B3-46FDF155FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ObservedStageDates" sheetId="2" r:id="rId1"/>
-    <sheet name="Observed" sheetId="1" r:id="rId2"/>
+    <sheet name="Observed" sheetId="1" r:id="rId1"/>
+    <sheet name="ObservedStageDates" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Observed!$A$1:$U$1283</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$U$1283</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -29016,678 +29016,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B26F740-CF2D-4018-B7F5-F37997C29FFA}">
-  <dimension ref="A3:F34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:F34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44312</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44446</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44499</v>
-      </c>
-      <c r="E5" s="1">
-        <v>44514</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1">
-        <v>44313</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44453</v>
-      </c>
-      <c r="D6" s="1">
-        <v>44499</v>
-      </c>
-      <c r="E6" s="1">
-        <v>44514</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44313</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44453</v>
-      </c>
-      <c r="D7" s="1">
-        <v>44499</v>
-      </c>
-      <c r="E7" s="1">
-        <v>44515</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44314</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44446</v>
-      </c>
-      <c r="D8" s="1">
-        <v>44499</v>
-      </c>
-      <c r="E8" s="1">
-        <v>44514</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="1">
-        <v>44285</v>
-      </c>
-      <c r="C9" s="1">
-        <v>44361</v>
-      </c>
-      <c r="D9" s="1">
-        <v>44484</v>
-      </c>
-      <c r="E9" s="1">
-        <v>44510</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1">
-        <v>44278</v>
-      </c>
-      <c r="C10" s="1">
-        <v>44361</v>
-      </c>
-      <c r="D10" s="1">
-        <v>44484</v>
-      </c>
-      <c r="E10" s="1">
-        <v>44512</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44281</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44361</v>
-      </c>
-      <c r="D11" s="1">
-        <v>44484</v>
-      </c>
-      <c r="E11" s="1">
-        <v>44510</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="1">
-        <v>44263</v>
-      </c>
-      <c r="C12" s="1">
-        <v>44346</v>
-      </c>
-      <c r="D12" s="1">
-        <v>44484</v>
-      </c>
-      <c r="E12" s="1">
-        <v>44507</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="1">
-        <v>44257</v>
-      </c>
-      <c r="C13" s="1">
-        <v>44346</v>
-      </c>
-      <c r="D13" s="1">
-        <v>44484</v>
-      </c>
-      <c r="E13" s="1">
-        <v>44509</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44257</v>
-      </c>
-      <c r="C14" s="1">
-        <v>44346</v>
-      </c>
-      <c r="D14" s="1">
-        <v>44484</v>
-      </c>
-      <c r="E14" s="1">
-        <v>44499</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1">
-        <v>44362</v>
-      </c>
-      <c r="C15" s="1">
-        <v>44467</v>
-      </c>
-      <c r="D15" s="1">
-        <v>44503</v>
-      </c>
-      <c r="E15" s="1">
-        <v>44517</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1">
-        <v>44362</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44471</v>
-      </c>
-      <c r="D16" s="1">
-        <v>44508</v>
-      </c>
-      <c r="E16" s="1">
-        <v>44523</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="1">
-        <v>44361</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44471</v>
-      </c>
-      <c r="D17" s="1">
-        <v>44503</v>
-      </c>
-      <c r="E17" s="1">
-        <v>44529</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
-        <v>44361</v>
-      </c>
-      <c r="C18" s="1">
-        <v>44471</v>
-      </c>
-      <c r="D18" s="1">
-        <v>44503</v>
-      </c>
-      <c r="E18" s="1">
-        <v>44529</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
-        <f>A5</f>
-        <v>Lincoln2021SD15AprCVCRW247</v>
-      </c>
-      <c r="B21" s="5">
-        <f>B5</f>
-        <v>44312</v>
-      </c>
-      <c r="C21" s="5">
-        <f t="shared" ref="C21:D21" si="0">C5</f>
-        <v>44446</v>
-      </c>
-      <c r="D21" s="5">
-        <f t="shared" si="0"/>
-        <v>44499</v>
-      </c>
-      <c r="E21" s="5">
-        <f t="shared" ref="E21:E34" si="1">ROUND(D21+(F21-D21)*0.8,0)</f>
-        <v>44511</v>
-      </c>
-      <c r="F21" s="5">
-        <f t="shared" ref="F21:F34" si="2">E5</f>
-        <v>44514</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
-        <f t="shared" ref="A22:D34" si="3">A6</f>
-        <v>Lincoln2021SD15AprCVGraham</v>
-      </c>
-      <c r="B22" s="5">
-        <f t="shared" si="3"/>
-        <v>44313</v>
-      </c>
-      <c r="C22" s="5">
-        <f t="shared" si="3"/>
-        <v>44453</v>
-      </c>
-      <c r="D22" s="5">
-        <f t="shared" si="3"/>
-        <v>44499</v>
-      </c>
-      <c r="E22" s="5">
-        <f t="shared" si="1"/>
-        <v>44511</v>
-      </c>
-      <c r="F22" s="5">
-        <f t="shared" si="2"/>
-        <v>44514</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD15AprCVKerrin</v>
-      </c>
-      <c r="B23" s="5">
-        <f t="shared" si="3"/>
-        <v>44313</v>
-      </c>
-      <c r="C23" s="5">
-        <f t="shared" si="3"/>
-        <v>44453</v>
-      </c>
-      <c r="D23" s="5">
-        <f t="shared" si="3"/>
-        <v>44499</v>
-      </c>
-      <c r="E23" s="5">
-        <f t="shared" si="1"/>
-        <v>44512</v>
-      </c>
-      <c r="F23" s="5">
-        <f t="shared" si="2"/>
-        <v>44515</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD15AprCVZyatt</v>
-      </c>
-      <c r="B24" s="5">
-        <f t="shared" si="3"/>
-        <v>44314</v>
-      </c>
-      <c r="C24" s="5">
-        <f t="shared" si="3"/>
-        <v>44446</v>
-      </c>
-      <c r="D24" s="5">
-        <f t="shared" si="3"/>
-        <v>44499</v>
-      </c>
-      <c r="E24" s="5">
-        <f t="shared" si="1"/>
-        <v>44511</v>
-      </c>
-      <c r="F24" s="5">
-        <f t="shared" si="2"/>
-        <v>44514</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD15MarCVGraham</v>
-      </c>
-      <c r="B25" s="5">
-        <f t="shared" si="3"/>
-        <v>44285</v>
-      </c>
-      <c r="C25" s="5">
-        <f t="shared" si="3"/>
-        <v>44361</v>
-      </c>
-      <c r="D25" s="5">
-        <f t="shared" si="3"/>
-        <v>44484</v>
-      </c>
-      <c r="E25" s="5">
-        <f t="shared" si="1"/>
-        <v>44505</v>
-      </c>
-      <c r="F25" s="5">
-        <f t="shared" si="2"/>
-        <v>44510</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD15MarCVKerrin</v>
-      </c>
-      <c r="B26" s="5">
-        <f t="shared" si="3"/>
-        <v>44278</v>
-      </c>
-      <c r="C26" s="5">
-        <f t="shared" si="3"/>
-        <v>44361</v>
-      </c>
-      <c r="D26" s="5">
-        <f t="shared" si="3"/>
-        <v>44484</v>
-      </c>
-      <c r="E26" s="5">
-        <f t="shared" si="1"/>
-        <v>44506</v>
-      </c>
-      <c r="F26" s="5">
-        <f t="shared" si="2"/>
-        <v>44512</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD15MarCVZyatt</v>
-      </c>
-      <c r="B27" s="5">
-        <f t="shared" si="3"/>
-        <v>44281</v>
-      </c>
-      <c r="C27" s="5">
-        <f t="shared" si="3"/>
-        <v>44361</v>
-      </c>
-      <c r="D27" s="5">
-        <f t="shared" si="3"/>
-        <v>44484</v>
-      </c>
-      <c r="E27" s="5">
-        <f t="shared" si="1"/>
-        <v>44505</v>
-      </c>
-      <c r="F27" s="5">
-        <f t="shared" si="2"/>
-        <v>44510</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD18FebCVGraham</v>
-      </c>
-      <c r="B28" s="5">
-        <f t="shared" si="3"/>
-        <v>44263</v>
-      </c>
-      <c r="C28" s="5">
-        <f t="shared" si="3"/>
-        <v>44346</v>
-      </c>
-      <c r="D28" s="5">
-        <f t="shared" si="3"/>
-        <v>44484</v>
-      </c>
-      <c r="E28" s="5">
-        <f t="shared" si="1"/>
-        <v>44502</v>
-      </c>
-      <c r="F28" s="5">
-        <f t="shared" si="2"/>
-        <v>44507</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD18FebCVKerrin</v>
-      </c>
-      <c r="B29" s="5">
-        <f t="shared" si="3"/>
-        <v>44257</v>
-      </c>
-      <c r="C29" s="5">
-        <f t="shared" si="3"/>
-        <v>44346</v>
-      </c>
-      <c r="D29" s="5">
-        <f t="shared" si="3"/>
-        <v>44484</v>
-      </c>
-      <c r="E29" s="5">
-        <f t="shared" si="1"/>
-        <v>44504</v>
-      </c>
-      <c r="F29" s="5">
-        <f t="shared" si="2"/>
-        <v>44509</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD18FebCVZyatt</v>
-      </c>
-      <c r="B30" s="5">
-        <f t="shared" si="3"/>
-        <v>44257</v>
-      </c>
-      <c r="C30" s="5">
-        <f t="shared" si="3"/>
-        <v>44346</v>
-      </c>
-      <c r="D30" s="5">
-        <f t="shared" si="3"/>
-        <v>44484</v>
-      </c>
-      <c r="E30" s="5">
-        <f t="shared" si="1"/>
-        <v>44496</v>
-      </c>
-      <c r="F30" s="5">
-        <f t="shared" si="2"/>
-        <v>44499</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD27MayCVCRW247</v>
-      </c>
-      <c r="B31" s="5">
-        <f t="shared" si="3"/>
-        <v>44362</v>
-      </c>
-      <c r="C31" s="5">
-        <f t="shared" si="3"/>
-        <v>44467</v>
-      </c>
-      <c r="D31" s="5">
-        <f t="shared" si="3"/>
-        <v>44503</v>
-      </c>
-      <c r="E31" s="5">
-        <f t="shared" si="1"/>
-        <v>44514</v>
-      </c>
-      <c r="F31" s="5">
-        <f t="shared" si="2"/>
-        <v>44517</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD27MayCVGraham</v>
-      </c>
-      <c r="B32" s="5">
-        <f t="shared" si="3"/>
-        <v>44362</v>
-      </c>
-      <c r="C32" s="5">
-        <f t="shared" si="3"/>
-        <v>44471</v>
-      </c>
-      <c r="D32" s="5">
-        <f t="shared" si="3"/>
-        <v>44508</v>
-      </c>
-      <c r="E32" s="5">
-        <f t="shared" si="1"/>
-        <v>44520</v>
-      </c>
-      <c r="F32" s="5">
-        <f t="shared" si="2"/>
-        <v>44523</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD27MayCVKerrin</v>
-      </c>
-      <c r="B33" s="5">
-        <f t="shared" si="3"/>
-        <v>44361</v>
-      </c>
-      <c r="C33" s="5">
-        <f t="shared" si="3"/>
-        <v>44471</v>
-      </c>
-      <c r="D33" s="5">
-        <f t="shared" si="3"/>
-        <v>44503</v>
-      </c>
-      <c r="E33" s="5">
-        <f t="shared" si="1"/>
-        <v>44524</v>
-      </c>
-      <c r="F33" s="5">
-        <f t="shared" si="2"/>
-        <v>44529</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="str">
-        <f t="shared" si="3"/>
-        <v>Lincoln2021SD27MayCVZyatt</v>
-      </c>
-      <c r="B34" s="5">
-        <f t="shared" si="3"/>
-        <v>44361</v>
-      </c>
-      <c r="C34" s="5">
-        <f t="shared" si="3"/>
-        <v>44471</v>
-      </c>
-      <c r="D34" s="5">
-        <f t="shared" si="3"/>
-        <v>44503</v>
-      </c>
-      <c r="E34" s="5">
-        <f t="shared" si="1"/>
-        <v>44524</v>
-      </c>
-      <c r="F34" s="5">
-        <f t="shared" si="2"/>
-        <v>44529</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1283"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -46187,4 +45519,672 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B26F740-CF2D-4018-B7F5-F37997C29FFA}">
+  <dimension ref="A3:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44312</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44446</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44499</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44313</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44453</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44499</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44313</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44453</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44499</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44515</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44314</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44446</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44499</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44514</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44285</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44361</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44484</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44510</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44278</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44361</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44484</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44512</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44281</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44361</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44484</v>
+      </c>
+      <c r="E11" s="1">
+        <v>44510</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44263</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44346</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44484</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44507</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44346</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44484</v>
+      </c>
+      <c r="E13" s="1">
+        <v>44509</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44257</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44346</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44484</v>
+      </c>
+      <c r="E14" s="1">
+        <v>44499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44362</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44467</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44503</v>
+      </c>
+      <c r="E15" s="1">
+        <v>44517</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44362</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44471</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44508</v>
+      </c>
+      <c r="E16" s="1">
+        <v>44523</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44361</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44471</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44503</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44529</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44361</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44471</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44503</v>
+      </c>
+      <c r="E18" s="1">
+        <v>44529</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>A5</f>
+        <v>Lincoln2021SD15AprCVCRW247</v>
+      </c>
+      <c r="B21" s="5">
+        <f>B5</f>
+        <v>44312</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" ref="C21:D21" si="0">C5</f>
+        <v>44446</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>44499</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" ref="E21:E34" si="1">ROUND(D21+(F21-D21)*0.8,0)</f>
+        <v>44511</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" ref="F21:F34" si="2">E5</f>
+        <v>44514</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" ref="A22:D34" si="3">A6</f>
+        <v>Lincoln2021SD15AprCVGraham</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" si="3"/>
+        <v>44313</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="3"/>
+        <v>44453</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="3"/>
+        <v>44499</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>44511</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="2"/>
+        <v>44514</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD15AprCVKerrin</v>
+      </c>
+      <c r="B23" s="5">
+        <f t="shared" si="3"/>
+        <v>44313</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="3"/>
+        <v>44453</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="3"/>
+        <v>44499</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>44512</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="2"/>
+        <v>44515</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD15AprCVZyatt</v>
+      </c>
+      <c r="B24" s="5">
+        <f t="shared" si="3"/>
+        <v>44314</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="3"/>
+        <v>44446</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="3"/>
+        <v>44499</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>44511</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="2"/>
+        <v>44514</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD15MarCVGraham</v>
+      </c>
+      <c r="B25" s="5">
+        <f t="shared" si="3"/>
+        <v>44285</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" si="3"/>
+        <v>44361</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="3"/>
+        <v>44484</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>44505</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="2"/>
+        <v>44510</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD15MarCVKerrin</v>
+      </c>
+      <c r="B26" s="5">
+        <f t="shared" si="3"/>
+        <v>44278</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" si="3"/>
+        <v>44361</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="3"/>
+        <v>44484</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="1"/>
+        <v>44506</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="2"/>
+        <v>44512</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD15MarCVZyatt</v>
+      </c>
+      <c r="B27" s="5">
+        <f t="shared" si="3"/>
+        <v>44281</v>
+      </c>
+      <c r="C27" s="5">
+        <f t="shared" si="3"/>
+        <v>44361</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="3"/>
+        <v>44484</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>44505</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="2"/>
+        <v>44510</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD18FebCVGraham</v>
+      </c>
+      <c r="B28" s="5">
+        <f t="shared" si="3"/>
+        <v>44263</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" si="3"/>
+        <v>44346</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="3"/>
+        <v>44484</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="1"/>
+        <v>44502</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="2"/>
+        <v>44507</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD18FebCVKerrin</v>
+      </c>
+      <c r="B29" s="5">
+        <f t="shared" si="3"/>
+        <v>44257</v>
+      </c>
+      <c r="C29" s="5">
+        <f t="shared" si="3"/>
+        <v>44346</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="3"/>
+        <v>44484</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="1"/>
+        <v>44504</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" si="2"/>
+        <v>44509</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD18FebCVZyatt</v>
+      </c>
+      <c r="B30" s="5">
+        <f t="shared" si="3"/>
+        <v>44257</v>
+      </c>
+      <c r="C30" s="5">
+        <f t="shared" si="3"/>
+        <v>44346</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="3"/>
+        <v>44484</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="1"/>
+        <v>44496</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="2"/>
+        <v>44499</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD27MayCVCRW247</v>
+      </c>
+      <c r="B31" s="5">
+        <f t="shared" si="3"/>
+        <v>44362</v>
+      </c>
+      <c r="C31" s="5">
+        <f t="shared" si="3"/>
+        <v>44467</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="3"/>
+        <v>44503</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="1"/>
+        <v>44514</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="2"/>
+        <v>44517</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD27MayCVGraham</v>
+      </c>
+      <c r="B32" s="5">
+        <f t="shared" si="3"/>
+        <v>44362</v>
+      </c>
+      <c r="C32" s="5">
+        <f t="shared" si="3"/>
+        <v>44471</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="3"/>
+        <v>44508</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="1"/>
+        <v>44520</v>
+      </c>
+      <c r="F32" s="5">
+        <f t="shared" si="2"/>
+        <v>44523</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD27MayCVKerrin</v>
+      </c>
+      <c r="B33" s="5">
+        <f t="shared" si="3"/>
+        <v>44361</v>
+      </c>
+      <c r="C33" s="5">
+        <f t="shared" si="3"/>
+        <v>44471</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="3"/>
+        <v>44503</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="1"/>
+        <v>44524</v>
+      </c>
+      <c r="F33" s="5">
+        <f t="shared" si="2"/>
+        <v>44529</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f t="shared" si="3"/>
+        <v>Lincoln2021SD27MayCVZyatt</v>
+      </c>
+      <c r="B34" s="5">
+        <f t="shared" si="3"/>
+        <v>44361</v>
+      </c>
+      <c r="C34" s="5">
+        <f t="shared" si="3"/>
+        <v>44471</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" si="3"/>
+        <v>44503</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" si="1"/>
+        <v>44524</v>
+      </c>
+      <c r="F34" s="5">
+        <f t="shared" si="2"/>
+        <v>44529</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>